<commit_message>
Make all parameter/variable names technology agnostic
</commit_message>
<xml_diff>
--- a/data/GAMS_input_demo.xlsx
+++ b/data/GAMS_input_demo.xlsx
@@ -8,26 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chrishun\Box Sync\YSSP_temp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B6ECF0-08D3-42DC-AA36-307D64771FAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A488E5DA-74E0-43B0-A990-5BED5D190915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9495" yWindow="-15660" windowWidth="23040" windowHeight="12315" tabRatio="705" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3480" yWindow="-21720" windowWidth="38640" windowHeight="21390" tabRatio="705" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="1" r:id="rId1"/>
     <sheet name="enr_glf_terms" sheetId="4" r:id="rId2"/>
     <sheet name="exog_tot_stock" sheetId="6" r:id="rId3"/>
     <sheet name="tec_add_gradient" sheetId="5" r:id="rId4"/>
-    <sheet name="recycle_rate" sheetId="7" r:id="rId5"/>
-    <sheet name="virg_mat_supply" sheetId="8" r:id="rId6"/>
-    <sheet name="mat_content" sheetId="9" r:id="rId7"/>
-    <sheet name="mat_impact_int" sheetId="10" r:id="rId8"/>
-    <sheet name="batt_portfolio" sheetId="14" r:id="rId9"/>
-    <sheet name="newtec_int_shr" sheetId="2" r:id="rId10"/>
-    <sheet name="eur_batt_share" sheetId="12" r:id="rId11"/>
-    <sheet name="manuf_cnstrnt" sheetId="11" r:id="rId12"/>
-    <sheet name="occupancy_rate" sheetId="3" r:id="rId13"/>
-    <sheet name="tec_parameters_raw" sheetId="15" r:id="rId14"/>
-    <sheet name="enr_tec_correspondance" sheetId="16" r:id="rId15"/>
+    <sheet name="collection_rate" sheetId="17" r:id="rId5"/>
+    <sheet name="recycle_rate" sheetId="7" r:id="rId6"/>
+    <sheet name="virg_mat_supply" sheetId="8" r:id="rId7"/>
+    <sheet name="mat_content" sheetId="9" r:id="rId8"/>
+    <sheet name="mat_impact_int" sheetId="10" r:id="rId9"/>
+    <sheet name="batt_portfolio" sheetId="14" r:id="rId10"/>
+    <sheet name="newtec_int_shr" sheetId="2" r:id="rId11"/>
+    <sheet name="eur_batt_share" sheetId="12" r:id="rId12"/>
+    <sheet name="manuf_cnstrnt" sheetId="11" r:id="rId13"/>
+    <sheet name="occupancy_rate" sheetId="3" r:id="rId14"/>
+    <sheet name="tec_parameters_raw" sheetId="15" r:id="rId15"/>
+    <sheet name="enr_tec_correspondance" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -77,7 +78,7 @@
     <author>Christine Hung</author>
   </authors>
   <commentList>
-    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0D00-000001000000}">
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0D00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -138,7 +139,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="58">
   <si>
     <t>bev_int_shr</t>
   </si>
@@ -309,6 +310,9 @@
   </si>
   <si>
     <t>newtec</t>
+  </si>
+  <si>
+    <t>collection_rate</t>
   </si>
 </sst>
 </file>
@@ -551,7 +555,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -580,7 +584,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -589,7 +592,6 @@
     <xf numFmtId="11" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -1272,38 +1274,38 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A30" s="30" t="s">
+      <c r="A30" s="29" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A31" s="31" t="s">
+      <c r="A31" s="30" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A32" s="31" t="s">
+      <c r="A32" s="30" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="32"/>
+      <c r="A33" s="31"/>
     </row>
     <row r="34" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A34" s="31" t="s">
+      <c r="A34" s="30" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="32"/>
+      <c r="A35" s="31"/>
     </row>
     <row r="36" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A36" s="31" t="s">
+      <c r="A36" s="30" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A37" s="31" t="s">
+      <c r="A37" s="30" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1315,6 +1317,570 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:N21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:R1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="16"/>
+    <col min="2" max="2" width="9.7109375" style="16" customWidth="1"/>
+    <col min="3" max="3" width="15" style="16" customWidth="1"/>
+    <col min="4" max="4" width="12" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" style="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="21"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="49"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="41">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="D3" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="19">
+        <v>2197</v>
+      </c>
+      <c r="F3" s="19">
+        <v>1.88</v>
+      </c>
+      <c r="G3" s="51">
+        <v>188.72813508993531</v>
+      </c>
+      <c r="J3" s="21"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="49"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="21"/>
+      <c r="B4" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="41">
+        <v>26.6</v>
+      </c>
+      <c r="D4" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="40">
+        <v>2795</v>
+      </c>
+      <c r="F4">
+        <v>2.41</v>
+      </c>
+      <c r="G4" s="52">
+        <v>259.37886848165812</v>
+      </c>
+      <c r="I4" s="16"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="49"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="21"/>
+      <c r="B5" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="41">
+        <v>42.2</v>
+      </c>
+      <c r="D5" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="40">
+        <v>4106</v>
+      </c>
+      <c r="F5">
+        <v>3.86</v>
+      </c>
+      <c r="G5" s="52">
+        <v>379.61240300552259</v>
+      </c>
+      <c r="I5" s="16"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="40"/>
+      <c r="N5" s="49"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="21"/>
+      <c r="B6" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="41">
+        <v>26.6</v>
+      </c>
+      <c r="D6" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="40">
+        <v>2795</v>
+      </c>
+      <c r="F6">
+        <v>2.41</v>
+      </c>
+      <c r="G6" s="52">
+        <v>259.37886848165812</v>
+      </c>
+      <c r="I6" s="16"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="40"/>
+      <c r="N6" s="49"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="21"/>
+      <c r="B7" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="41">
+        <v>42.2</v>
+      </c>
+      <c r="D7" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="40">
+        <v>4106</v>
+      </c>
+      <c r="F7">
+        <v>3.86</v>
+      </c>
+      <c r="G7" s="52">
+        <v>379.61240300552259</v>
+      </c>
+      <c r="I7" s="16"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="40"/>
+      <c r="L7" s="40"/>
+      <c r="M7" s="40"/>
+      <c r="N7" s="49"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="21"/>
+      <c r="B8" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="41">
+        <v>26.6</v>
+      </c>
+      <c r="D8" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="40">
+        <v>2795</v>
+      </c>
+      <c r="F8">
+        <v>2.41</v>
+      </c>
+      <c r="G8" s="52">
+        <v>259.37886848165812</v>
+      </c>
+      <c r="I8" s="16"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="40"/>
+      <c r="L8" s="40"/>
+      <c r="M8" s="40"/>
+      <c r="N8" s="49"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="21"/>
+      <c r="B9" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="41">
+        <v>42.2</v>
+      </c>
+      <c r="D9" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="40">
+        <v>4106</v>
+      </c>
+      <c r="F9">
+        <v>3.86</v>
+      </c>
+      <c r="G9" s="52">
+        <v>379.61240300552259</v>
+      </c>
+      <c r="I9" s="16"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="40"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="40"/>
+      <c r="N9" s="49"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="21"/>
+      <c r="B10" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="41">
+        <v>59.9</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="40">
+        <v>7000</v>
+      </c>
+      <c r="F10">
+        <v>5.17</v>
+      </c>
+      <c r="G10" s="52">
+        <v>506.94546978896818</v>
+      </c>
+      <c r="I10" s="16"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="40"/>
+      <c r="L10" s="40"/>
+      <c r="M10" s="40"/>
+      <c r="N10" s="49"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="21"/>
+      <c r="B11" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="41">
+        <v>59.9</v>
+      </c>
+      <c r="D11" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="40">
+        <v>7000</v>
+      </c>
+      <c r="F11">
+        <v>5.17</v>
+      </c>
+      <c r="G11" s="52">
+        <v>506.94546978896818</v>
+      </c>
+      <c r="I11" s="16"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="40"/>
+      <c r="L11" s="40"/>
+      <c r="M11" s="40"/>
+      <c r="N11" s="49"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="21"/>
+      <c r="B12" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="41">
+        <v>75</v>
+      </c>
+      <c r="D12" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="40">
+        <v>8191</v>
+      </c>
+      <c r="F12">
+        <v>6.95</v>
+      </c>
+      <c r="G12" s="52">
+        <v>684.27360431283273</v>
+      </c>
+      <c r="I12" s="16"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="40"/>
+      <c r="L12" s="40"/>
+      <c r="M12" s="40"/>
+      <c r="N12" s="49"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="21"/>
+      <c r="B13" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="41">
+        <v>75</v>
+      </c>
+      <c r="D13" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="40">
+        <v>8191</v>
+      </c>
+      <c r="F13">
+        <v>6.95</v>
+      </c>
+      <c r="G13" s="52">
+        <v>684.27360431283273</v>
+      </c>
+      <c r="I13" s="16"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="40"/>
+      <c r="L13" s="40"/>
+      <c r="M13" s="40"/>
+      <c r="N13" s="49"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="21"/>
+      <c r="B14" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="41">
+        <v>89.8</v>
+      </c>
+      <c r="D14" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="40">
+        <v>11900</v>
+      </c>
+      <c r="F14">
+        <v>7.63</v>
+      </c>
+      <c r="G14" s="52">
+        <v>740.03953883669703</v>
+      </c>
+      <c r="I14" s="16"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="40"/>
+      <c r="L14" s="40"/>
+      <c r="M14" s="40"/>
+      <c r="N14" s="49"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="21"/>
+      <c r="B15" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="41">
+        <v>95</v>
+      </c>
+      <c r="D15" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="40">
+        <v>12453</v>
+      </c>
+      <c r="F15">
+        <v>7.87</v>
+      </c>
+      <c r="G15" s="52">
+        <v>856.08018367798525</v>
+      </c>
+      <c r="I15" s="16"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="40"/>
+      <c r="L15" s="40"/>
+      <c r="M15" s="40"/>
+      <c r="N15" s="49"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="21"/>
+      <c r="B16" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="41">
+        <v>100</v>
+      </c>
+      <c r="D16" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="40">
+        <v>13566</v>
+      </c>
+      <c r="F16">
+        <v>8.4499999999999993</v>
+      </c>
+      <c r="G16" s="52">
+        <v>837.373293546117</v>
+      </c>
+      <c r="I16" s="16"/>
+      <c r="J16" s="21"/>
+      <c r="K16" s="40"/>
+      <c r="L16" s="40"/>
+      <c r="M16" s="40"/>
+      <c r="N16" s="49"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="21"/>
+      <c r="B17" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="41">
+        <v>89.8</v>
+      </c>
+      <c r="D17" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="40">
+        <v>11900</v>
+      </c>
+      <c r="F17">
+        <v>7.63</v>
+      </c>
+      <c r="G17" s="52">
+        <v>740.03953883669703</v>
+      </c>
+      <c r="I17" s="16"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="40"/>
+      <c r="L17" s="40"/>
+      <c r="M17" s="40"/>
+      <c r="N17" s="49"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="21"/>
+      <c r="B18" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="41">
+        <v>95</v>
+      </c>
+      <c r="D18" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="40">
+        <v>12453</v>
+      </c>
+      <c r="F18">
+        <v>7.87</v>
+      </c>
+      <c r="G18" s="52">
+        <v>856.08018367798525</v>
+      </c>
+      <c r="I18" s="16"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="40"/>
+      <c r="L18" s="40"/>
+      <c r="M18" s="40"/>
+      <c r="N18" s="49"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="21"/>
+      <c r="B19" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="41">
+        <v>100</v>
+      </c>
+      <c r="D19" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" s="40">
+        <v>13566</v>
+      </c>
+      <c r="F19">
+        <v>8.4499999999999993</v>
+      </c>
+      <c r="G19" s="52">
+        <v>837.373293546117</v>
+      </c>
+      <c r="I19" s="16"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="40"/>
+      <c r="L19" s="40"/>
+      <c r="M19" s="40"/>
+      <c r="N19" s="49"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="21"/>
+      <c r="B20" s="41" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="41">
+        <v>89.8</v>
+      </c>
+      <c r="D20" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="40">
+        <v>11900</v>
+      </c>
+      <c r="F20">
+        <v>7.63</v>
+      </c>
+      <c r="G20" s="52">
+        <v>740.03953883669703</v>
+      </c>
+      <c r="I20" s="16"/>
+      <c r="K20" s="16"/>
+    </row>
+    <row r="21" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="22"/>
+      <c r="B21" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="44">
+        <v>95</v>
+      </c>
+      <c r="D21" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" s="23">
+        <v>12453</v>
+      </c>
+      <c r="F21" s="23">
+        <v>7.87</v>
+      </c>
+      <c r="G21" s="53">
+        <v>856.08018367798525</v>
+      </c>
+      <c r="I21" s="16"/>
+      <c r="K21" s="16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
@@ -1342,7 +1908,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
@@ -1369,7 +1935,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
@@ -1984,7 +2550,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
@@ -2012,15 +2578,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R52" sqref="R52"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R67" sqref="R67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2061,83 +2627,83 @@
       <c r="A3" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="48"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="50">
+      <c r="E3" s="46"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="48">
         <v>1400</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="21"/>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42" t="s">
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="51"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="44">
+      <c r="E4" s="49"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="42">
         <v>1650</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="21"/>
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42" t="s">
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="51"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="44">
+      <c r="E5" s="49"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="42">
         <v>1900</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="21"/>
-      <c r="B6" s="42"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42" t="s">
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="51"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="44">
+      <c r="E6" s="49"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="42">
         <v>2220</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="21"/>
-      <c r="B7" s="42"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42" t="s">
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="51"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="44">
+      <c r="E7" s="49"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="42">
         <v>1400</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="21"/>
-      <c r="B8" s="42"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42" t="s">
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="51"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="44">
+      <c r="E8" s="49"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="42">
         <v>2700</v>
       </c>
     </row>
@@ -2145,167 +2711,167 @@
       <c r="A9" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="42" t="s">
+      <c r="D9" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="51">
+      <c r="E9" s="49">
         <v>3000</v>
       </c>
-      <c r="F9" s="43"/>
-      <c r="G9" s="44"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="42"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="21"/>
-      <c r="B10" s="42"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42" t="s">
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="51">
+      <c r="E10" s="49">
         <v>3800</v>
       </c>
-      <c r="F10" s="43"/>
-      <c r="G10" s="44"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="42"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="21"/>
-      <c r="B11" s="42"/>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42" t="s">
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="51">
+      <c r="E11" s="49">
         <v>4900</v>
       </c>
-      <c r="F11" s="43"/>
-      <c r="G11" s="44"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="42"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="21"/>
-      <c r="B12" s="42"/>
-      <c r="C12" s="42"/>
-      <c r="D12" s="42" t="s">
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="51">
+      <c r="E12" s="49">
         <v>6800</v>
       </c>
-      <c r="F12" s="43"/>
-      <c r="G12" s="44"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="42"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="21"/>
-      <c r="B13" s="42"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="42" t="s">
+      <c r="B13" s="40"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="51">
+      <c r="E13" s="49">
         <v>7800</v>
       </c>
-      <c r="F13" s="43"/>
-      <c r="G13" s="44"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="42"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="21"/>
-      <c r="B14" s="42"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="42" t="s">
+      <c r="B14" s="40"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="51">
+      <c r="E14" s="49">
         <v>9100</v>
       </c>
-      <c r="F14" s="43"/>
-      <c r="G14" s="44"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="42"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="42" t="s">
+      <c r="B15" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="42" t="s">
+      <c r="C15" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="42" t="s">
+      <c r="D15" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="51"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="44">
+      <c r="E15" s="49"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="42">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="21"/>
-      <c r="B16" s="42"/>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42" t="s">
+      <c r="B16" s="40"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="51"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="44">
+      <c r="E16" s="49"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="42">
         <v>5.75</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="21"/>
-      <c r="B17" s="42"/>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42" t="s">
+      <c r="B17" s="40"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="51"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="44">
+      <c r="E17" s="49"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="42">
         <v>6.8</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="21"/>
-      <c r="B18" s="42"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42" t="s">
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="51"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="44">
+      <c r="E18" s="49"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="42">
         <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="21"/>
-      <c r="B19" s="42"/>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42" t="s">
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="51"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="44">
+      <c r="E19" s="49"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="42">
         <v>8.5</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="21"/>
-      <c r="B20" s="42"/>
-      <c r="C20" s="42"/>
-      <c r="D20" s="42" t="s">
+      <c r="B20" s="40"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="E20" s="51"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="44">
+      <c r="E20" s="49"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="42">
         <v>9.6</v>
       </c>
     </row>
@@ -2313,179 +2879,179 @@
       <c r="A21" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="42" t="s">
+      <c r="B21" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="42" t="s">
+      <c r="C21" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="42" t="s">
+      <c r="D21" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="E21" s="51">
+      <c r="E21" s="49">
         <v>2.5</v>
       </c>
-      <c r="F21" s="43">
+      <c r="F21" s="41">
         <v>4.8</v>
       </c>
-      <c r="G21" s="44"/>
+      <c r="G21" s="42"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="21"/>
-      <c r="B22" s="42"/>
-      <c r="C22" s="42"/>
-      <c r="D22" s="42" t="s">
+      <c r="B22" s="40"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="E22" s="51">
+      <c r="E22" s="49">
         <v>3</v>
       </c>
-      <c r="F22" s="43">
+      <c r="F22" s="41">
         <v>5.5</v>
       </c>
-      <c r="G22" s="44"/>
+      <c r="G22" s="42"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="21"/>
-      <c r="B23" s="42"/>
-      <c r="C23" s="42"/>
-      <c r="D23" s="42" t="s">
+      <c r="B23" s="40"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="E23" s="51">
+      <c r="E23" s="49">
         <v>3.7</v>
       </c>
-      <c r="F23" s="43">
+      <c r="F23" s="41">
         <v>6.5</v>
       </c>
-      <c r="G23" s="44"/>
+      <c r="G23" s="42"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="21"/>
-      <c r="B24" s="42"/>
-      <c r="C24" s="42"/>
-      <c r="D24" s="42" t="s">
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="E24" s="51">
+      <c r="E24" s="49">
         <v>5</v>
       </c>
-      <c r="F24" s="43">
+      <c r="F24" s="41">
         <v>7</v>
       </c>
-      <c r="G24" s="44"/>
+      <c r="G24" s="42"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="21"/>
-      <c r="B25" s="42"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="42" t="s">
+      <c r="B25" s="40"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="E25" s="51">
+      <c r="E25" s="49">
         <v>6</v>
       </c>
-      <c r="F25" s="43">
+      <c r="F25" s="41">
         <v>7.5</v>
       </c>
-      <c r="G25" s="44"/>
+      <c r="G25" s="42"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="21"/>
-      <c r="B26" s="42"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="42" t="s">
+      <c r="B26" s="40"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="E26" s="51">
+      <c r="E26" s="49">
         <v>7</v>
       </c>
-      <c r="F26" s="43">
+      <c r="F26" s="41">
         <v>8</v>
       </c>
-      <c r="G26" s="44"/>
+      <c r="G26" s="42"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="42" t="s">
+      <c r="B27" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="42" t="s">
+      <c r="C27" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="D27" s="42" t="s">
+      <c r="D27" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="E27" s="51"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="45">
+      <c r="E27" s="49"/>
+      <c r="F27" s="41"/>
+      <c r="G27" s="43">
         <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="21"/>
-      <c r="B28" s="42"/>
-      <c r="C28" s="42"/>
-      <c r="D28" s="42" t="s">
+      <c r="B28" s="40"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="E28" s="51"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="45">
+      <c r="E28" s="49"/>
+      <c r="F28" s="41"/>
+      <c r="G28" s="43">
         <v>0.57499999999999996</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="21"/>
-      <c r="B29" s="42"/>
-      <c r="C29" s="42"/>
-      <c r="D29" s="42" t="s">
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="E29" s="51"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="45">
+      <c r="E29" s="49"/>
+      <c r="F29" s="41"/>
+      <c r="G29" s="43">
         <v>0.65</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="21"/>
-      <c r="B30" s="42"/>
-      <c r="C30" s="42"/>
-      <c r="D30" s="42" t="s">
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="E30" s="51"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="45">
+      <c r="E30" s="49"/>
+      <c r="F30" s="41"/>
+      <c r="G30" s="43">
         <v>0.7</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="21"/>
-      <c r="B31" s="42"/>
-      <c r="C31" s="42"/>
-      <c r="D31" s="42" t="s">
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="E31" s="51"/>
-      <c r="F31" s="43"/>
-      <c r="G31" s="45">
+      <c r="E31" s="49"/>
+      <c r="F31" s="41"/>
+      <c r="G31" s="43">
         <v>0.85</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="21"/>
-      <c r="B32" s="42"/>
-      <c r="C32" s="42"/>
-      <c r="D32" s="42" t="s">
+      <c r="B32" s="40"/>
+      <c r="C32" s="40"/>
+      <c r="D32" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="E32" s="51"/>
-      <c r="F32" s="43"/>
-      <c r="G32" s="45">
+      <c r="E32" s="49"/>
+      <c r="F32" s="41"/>
+      <c r="G32" s="43">
         <v>1</v>
       </c>
     </row>
@@ -2493,83 +3059,83 @@
       <c r="A33" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="B33" s="42" t="s">
+      <c r="B33" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="C33" s="42" t="s">
+      <c r="C33" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="D33" s="42" t="s">
+      <c r="D33" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="E33" s="51"/>
-      <c r="F33" s="43"/>
-      <c r="G33" s="44">
+      <c r="E33" s="49"/>
+      <c r="F33" s="41"/>
+      <c r="G33" s="42">
         <v>0.15</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="21"/>
-      <c r="B34" s="42"/>
-      <c r="C34" s="42"/>
-      <c r="D34" s="42" t="s">
+      <c r="B34" s="40"/>
+      <c r="C34" s="40"/>
+      <c r="D34" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="E34" s="51"/>
-      <c r="F34" s="43"/>
-      <c r="G34" s="44">
+      <c r="E34" s="49"/>
+      <c r="F34" s="41"/>
+      <c r="G34" s="42">
         <v>0.17499999999999999</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="21"/>
-      <c r="B35" s="42"/>
-      <c r="C35" s="42"/>
-      <c r="D35" s="42" t="s">
+      <c r="B35" s="40"/>
+      <c r="C35" s="40"/>
+      <c r="D35" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="E35" s="51"/>
-      <c r="F35" s="43"/>
-      <c r="G35" s="44">
+      <c r="E35" s="49"/>
+      <c r="F35" s="41"/>
+      <c r="G35" s="42">
         <v>0.18</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="21"/>
-      <c r="B36" s="42"/>
-      <c r="C36" s="42"/>
-      <c r="D36" s="42" t="s">
+      <c r="B36" s="40"/>
+      <c r="C36" s="40"/>
+      <c r="D36" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="E36" s="51"/>
-      <c r="F36" s="43"/>
-      <c r="G36" s="44">
+      <c r="E36" s="49"/>
+      <c r="F36" s="41"/>
+      <c r="G36" s="42">
         <v>0.2</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="21"/>
-      <c r="B37" s="42"/>
-      <c r="C37" s="42"/>
-      <c r="D37" s="42" t="s">
+      <c r="B37" s="40"/>
+      <c r="C37" s="40"/>
+      <c r="D37" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="E37" s="51"/>
-      <c r="F37" s="43"/>
-      <c r="G37" s="44">
+      <c r="E37" s="49"/>
+      <c r="F37" s="41"/>
+      <c r="G37" s="42">
         <v>0.21</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="21"/>
-      <c r="B38" s="42"/>
-      <c r="C38" s="42"/>
-      <c r="D38" s="42" t="s">
+      <c r="B38" s="40"/>
+      <c r="C38" s="40"/>
+      <c r="D38" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="E38" s="51"/>
-      <c r="F38" s="43"/>
-      <c r="G38" s="44">
+      <c r="E38" s="49"/>
+      <c r="F38" s="41"/>
+      <c r="G38" s="42">
         <v>0.22500000000000001</v>
       </c>
     </row>
@@ -2577,83 +3143,83 @@
       <c r="A39" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="B39" s="42" t="s">
+      <c r="B39" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="C39" s="42" t="s">
+      <c r="C39" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="D39" s="42" t="s">
+      <c r="D39" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="E39" s="51"/>
-      <c r="F39" s="43"/>
-      <c r="G39" s="44">
+      <c r="E39" s="49"/>
+      <c r="F39" s="41"/>
+      <c r="G39" s="42">
         <v>0.3</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="21"/>
-      <c r="B40" s="42"/>
-      <c r="C40" s="42"/>
-      <c r="D40" s="42" t="s">
+      <c r="B40" s="40"/>
+      <c r="C40" s="40"/>
+      <c r="D40" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="E40" s="51"/>
-      <c r="F40" s="43"/>
-      <c r="G40" s="44">
+      <c r="E40" s="49"/>
+      <c r="F40" s="41"/>
+      <c r="G40" s="42">
         <v>0.35</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="21"/>
-      <c r="B41" s="42"/>
-      <c r="C41" s="42"/>
-      <c r="D41" s="42" t="s">
+      <c r="B41" s="40"/>
+      <c r="C41" s="40"/>
+      <c r="D41" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="E41" s="51"/>
-      <c r="F41" s="43"/>
-      <c r="G41" s="44">
+      <c r="E41" s="49"/>
+      <c r="F41" s="41"/>
+      <c r="G41" s="42">
         <v>0.5</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="21"/>
-      <c r="B42" s="42"/>
-      <c r="C42" s="42"/>
-      <c r="D42" s="42" t="s">
+      <c r="B42" s="40"/>
+      <c r="C42" s="40"/>
+      <c r="D42" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="E42" s="51"/>
-      <c r="F42" s="43"/>
-      <c r="G42" s="44">
+      <c r="E42" s="49"/>
+      <c r="F42" s="41"/>
+      <c r="G42" s="42">
         <v>0.6</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="21"/>
-      <c r="B43" s="42"/>
-      <c r="C43" s="42"/>
-      <c r="D43" s="42" t="s">
+      <c r="B43" s="40"/>
+      <c r="C43" s="40"/>
+      <c r="D43" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="E43" s="51"/>
-      <c r="F43" s="43"/>
-      <c r="G43" s="44">
+      <c r="E43" s="49"/>
+      <c r="F43" s="41"/>
+      <c r="G43" s="42">
         <v>0.65</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="21"/>
-      <c r="B44" s="42"/>
-      <c r="C44" s="42"/>
-      <c r="D44" s="42" t="s">
+      <c r="B44" s="40"/>
+      <c r="C44" s="40"/>
+      <c r="D44" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="E44" s="51"/>
-      <c r="F44" s="43"/>
-      <c r="G44" s="44">
+      <c r="E44" s="49"/>
+      <c r="F44" s="41"/>
+      <c r="G44" s="42">
         <v>0.7</v>
       </c>
     </row>
@@ -2661,70 +3227,70 @@
       <c r="A45" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="B45" s="42" t="s">
+      <c r="B45" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="C45" s="42" t="s">
+      <c r="C45" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="D45" s="42" t="s">
+      <c r="D45" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="E45" s="51"/>
-      <c r="F45" s="43"/>
-      <c r="G45" s="44">
+      <c r="E45" s="49"/>
+      <c r="F45" s="41"/>
+      <c r="G45" s="42">
         <v>0.5</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="21"/>
-      <c r="B46" s="42"/>
-      <c r="C46" s="42"/>
-      <c r="D46" s="42" t="s">
+      <c r="B46" s="40"/>
+      <c r="C46" s="40"/>
+      <c r="D46" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="E46" s="51"/>
-      <c r="F46" s="43"/>
-      <c r="G46" s="44">
+      <c r="E46" s="49"/>
+      <c r="F46" s="41"/>
+      <c r="G46" s="42">
         <v>0.6</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="21"/>
-      <c r="B47" s="42"/>
-      <c r="C47" s="42"/>
-      <c r="D47" s="42" t="s">
+      <c r="B47" s="40"/>
+      <c r="C47" s="40"/>
+      <c r="D47" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="E47" s="51"/>
-      <c r="F47" s="43"/>
-      <c r="G47" s="44">
+      <c r="E47" s="49"/>
+      <c r="F47" s="41"/>
+      <c r="G47" s="42">
         <v>0.7</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="21"/>
-      <c r="B48" s="42"/>
-      <c r="C48" s="42"/>
-      <c r="D48" s="42" t="s">
+      <c r="B48" s="40"/>
+      <c r="C48" s="40"/>
+      <c r="D48" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="E48" s="51"/>
-      <c r="F48" s="43"/>
-      <c r="G48" s="44">
+      <c r="E48" s="49"/>
+      <c r="F48" s="41"/>
+      <c r="G48" s="42">
         <v>0.75</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="21"/>
-      <c r="B49" s="42"/>
-      <c r="C49" s="42"/>
-      <c r="D49" s="42" t="s">
+      <c r="B49" s="40"/>
+      <c r="C49" s="40"/>
+      <c r="D49" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="E49" s="51"/>
-      <c r="F49" s="43"/>
-      <c r="G49" s="44">
+      <c r="E49" s="49"/>
+      <c r="F49" s="41"/>
+      <c r="G49" s="42">
         <v>0.8</v>
       </c>
     </row>
@@ -2735,9 +3301,9 @@
       <c r="D50" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E50" s="52"/>
-      <c r="F50" s="46"/>
-      <c r="G50" s="47">
+      <c r="E50" s="50"/>
+      <c r="F50" s="44"/>
+      <c r="G50" s="45">
         <v>0.9</v>
       </c>
     </row>
@@ -2748,7 +3314,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <sheetPr codeName="Sheet16">
     <tabColor rgb="FFFFFF00"/>
@@ -2810,7 +3376,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2978,912 +3544,912 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" style="29" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" style="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:82" s="14" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29"/>
+      <c r="A1" s="28"/>
     </row>
     <row r="2" spans="1:82" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="38">
+      <c r="B2" s="36">
         <v>2000</v>
       </c>
-      <c r="C2" s="39">
+      <c r="C2" s="37">
         <v>2001</v>
       </c>
-      <c r="D2" s="39">
+      <c r="D2" s="37">
         <v>2002</v>
       </c>
-      <c r="E2" s="39">
+      <c r="E2" s="37">
         <v>2003</v>
       </c>
-      <c r="F2" s="39">
+      <c r="F2" s="37">
         <v>2004</v>
       </c>
-      <c r="G2" s="39">
+      <c r="G2" s="37">
         <v>2005</v>
       </c>
-      <c r="H2" s="39">
+      <c r="H2" s="37">
         <v>2006</v>
       </c>
-      <c r="I2" s="39">
+      <c r="I2" s="37">
         <v>2007</v>
       </c>
-      <c r="J2" s="39">
+      <c r="J2" s="37">
         <v>2008</v>
       </c>
-      <c r="K2" s="39">
+      <c r="K2" s="37">
         <v>2009</v>
       </c>
-      <c r="L2" s="39">
+      <c r="L2" s="37">
         <v>2010</v>
       </c>
-      <c r="M2" s="39">
+      <c r="M2" s="37">
         <v>2011</v>
       </c>
-      <c r="N2" s="39">
+      <c r="N2" s="37">
         <v>2012</v>
       </c>
-      <c r="O2" s="39">
+      <c r="O2" s="37">
         <v>2013</v>
       </c>
-      <c r="P2" s="39">
+      <c r="P2" s="37">
         <v>2014</v>
       </c>
-      <c r="Q2" s="39">
+      <c r="Q2" s="37">
         <v>2015</v>
       </c>
-      <c r="R2" s="39">
+      <c r="R2" s="37">
         <v>2016</v>
       </c>
-      <c r="S2" s="39">
+      <c r="S2" s="37">
         <v>2017</v>
       </c>
-      <c r="T2" s="39">
+      <c r="T2" s="37">
         <v>2018</v>
       </c>
-      <c r="U2" s="39">
+      <c r="U2" s="37">
         <v>2019</v>
       </c>
-      <c r="V2" s="39">
+      <c r="V2" s="37">
         <v>2020</v>
       </c>
-      <c r="W2" s="39">
+      <c r="W2" s="37">
         <v>2021</v>
       </c>
-      <c r="X2" s="39">
+      <c r="X2" s="37">
         <v>2022</v>
       </c>
-      <c r="Y2" s="39">
+      <c r="Y2" s="37">
         <v>2023</v>
       </c>
-      <c r="Z2" s="39">
+      <c r="Z2" s="37">
         <v>2024</v>
       </c>
-      <c r="AA2" s="39">
+      <c r="AA2" s="37">
         <v>2025</v>
       </c>
-      <c r="AB2" s="39">
+      <c r="AB2" s="37">
         <v>2026</v>
       </c>
-      <c r="AC2" s="39">
+      <c r="AC2" s="37">
         <v>2027</v>
       </c>
-      <c r="AD2" s="39">
+      <c r="AD2" s="37">
         <v>2028</v>
       </c>
-      <c r="AE2" s="39">
+      <c r="AE2" s="37">
         <v>2029</v>
       </c>
-      <c r="AF2" s="39">
+      <c r="AF2" s="37">
         <v>2030</v>
       </c>
-      <c r="AG2" s="39">
+      <c r="AG2" s="37">
         <v>2031</v>
       </c>
-      <c r="AH2" s="39">
+      <c r="AH2" s="37">
         <v>2032</v>
       </c>
-      <c r="AI2" s="39">
+      <c r="AI2" s="37">
         <v>2033</v>
       </c>
-      <c r="AJ2" s="39">
+      <c r="AJ2" s="37">
         <v>2034</v>
       </c>
-      <c r="AK2" s="39">
+      <c r="AK2" s="37">
         <v>2035</v>
       </c>
-      <c r="AL2" s="39">
+      <c r="AL2" s="37">
         <v>2036</v>
       </c>
-      <c r="AM2" s="39">
+      <c r="AM2" s="37">
         <v>2037</v>
       </c>
-      <c r="AN2" s="39">
+      <c r="AN2" s="37">
         <v>2038</v>
       </c>
-      <c r="AO2" s="39">
+      <c r="AO2" s="37">
         <v>2039</v>
       </c>
-      <c r="AP2" s="39">
+      <c r="AP2" s="37">
         <v>2040</v>
       </c>
-      <c r="AQ2" s="39">
+      <c r="AQ2" s="37">
         <v>2041</v>
       </c>
-      <c r="AR2" s="39">
+      <c r="AR2" s="37">
         <v>2042</v>
       </c>
-      <c r="AS2" s="39">
+      <c r="AS2" s="37">
         <v>2043</v>
       </c>
-      <c r="AT2" s="39">
+      <c r="AT2" s="37">
         <v>2044</v>
       </c>
-      <c r="AU2" s="39">
+      <c r="AU2" s="37">
         <v>2045</v>
       </c>
-      <c r="AV2" s="39">
+      <c r="AV2" s="37">
         <v>2046</v>
       </c>
-      <c r="AW2" s="39">
+      <c r="AW2" s="37">
         <v>2047</v>
       </c>
-      <c r="AX2" s="39">
+      <c r="AX2" s="37">
         <v>2048</v>
       </c>
-      <c r="AY2" s="39">
+      <c r="AY2" s="37">
         <v>2049</v>
       </c>
-      <c r="AZ2" s="39">
+      <c r="AZ2" s="37">
         <v>2050</v>
       </c>
-      <c r="BA2" s="40">
+      <c r="BA2" s="38">
         <v>2051</v>
       </c>
-      <c r="BB2" s="40">
+      <c r="BB2" s="38">
         <v>2052</v>
       </c>
-      <c r="BC2" s="40">
+      <c r="BC2" s="38">
         <v>2053</v>
       </c>
-      <c r="BD2" s="40">
+      <c r="BD2" s="38">
         <v>2054</v>
       </c>
-      <c r="BE2" s="40">
+      <c r="BE2" s="38">
         <v>2055</v>
       </c>
-      <c r="BF2" s="40">
+      <c r="BF2" s="38">
         <v>2056</v>
       </c>
-      <c r="BG2" s="40">
+      <c r="BG2" s="38">
         <v>2057</v>
       </c>
-      <c r="BH2" s="40">
+      <c r="BH2" s="38">
         <v>2058</v>
       </c>
-      <c r="BI2" s="40">
+      <c r="BI2" s="38">
         <v>2059</v>
       </c>
-      <c r="BJ2" s="40">
+      <c r="BJ2" s="38">
         <v>2060</v>
       </c>
-      <c r="BK2" s="40">
+      <c r="BK2" s="38">
         <v>2061</v>
       </c>
-      <c r="BL2" s="40">
+      <c r="BL2" s="38">
         <v>2062</v>
       </c>
-      <c r="BM2" s="40">
+      <c r="BM2" s="38">
         <v>2063</v>
       </c>
-      <c r="BN2" s="40">
+      <c r="BN2" s="38">
         <v>2064</v>
       </c>
-      <c r="BO2" s="40">
+      <c r="BO2" s="38">
         <v>2065</v>
       </c>
-      <c r="BP2" s="40">
+      <c r="BP2" s="38">
         <v>2066</v>
       </c>
-      <c r="BQ2" s="40">
+      <c r="BQ2" s="38">
         <v>2067</v>
       </c>
-      <c r="BR2" s="40">
+      <c r="BR2" s="38">
         <v>2068</v>
       </c>
-      <c r="BS2" s="40">
+      <c r="BS2" s="38">
         <v>2069</v>
       </c>
-      <c r="BT2" s="40">
+      <c r="BT2" s="38">
         <v>2070</v>
       </c>
-      <c r="BU2" s="40">
+      <c r="BU2" s="38">
         <v>2071</v>
       </c>
-      <c r="BV2" s="40">
+      <c r="BV2" s="38">
         <v>2072</v>
       </c>
-      <c r="BW2" s="40">
+      <c r="BW2" s="38">
         <v>2073</v>
       </c>
-      <c r="BX2" s="40">
+      <c r="BX2" s="38">
         <v>2074</v>
       </c>
-      <c r="BY2" s="40">
+      <c r="BY2" s="38">
         <v>2075</v>
       </c>
-      <c r="BZ2" s="40">
+      <c r="BZ2" s="38">
         <v>2076</v>
       </c>
-      <c r="CA2" s="40">
+      <c r="CA2" s="38">
         <v>2077</v>
       </c>
-      <c r="CB2" s="40">
+      <c r="CB2" s="38">
         <v>2078</v>
       </c>
-      <c r="CC2" s="40">
+      <c r="CC2" s="38">
         <v>2079</v>
       </c>
-      <c r="CD2" s="41">
+      <c r="CD2" s="39">
         <v>2080</v>
       </c>
     </row>
     <row r="3" spans="1:82" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="29">
+      <c r="B3" s="28">
         <f>C3/1.005-300</f>
         <v>271218.87127999583</v>
       </c>
-      <c r="C3" s="29">
+      <c r="C3" s="28">
         <f t="shared" ref="C3:U3" si="0">D3/1.005</f>
         <v>272876.46563639579</v>
       </c>
-      <c r="D3" s="29">
+      <c r="D3" s="28">
         <f t="shared" si="0"/>
         <v>274240.84796457773</v>
       </c>
-      <c r="E3" s="29">
+      <c r="E3" s="28">
         <f t="shared" si="0"/>
         <v>275612.05220440059</v>
       </c>
-      <c r="F3" s="29">
+      <c r="F3" s="28">
         <f t="shared" si="0"/>
         <v>276990.11246542254</v>
       </c>
-      <c r="G3" s="29">
+      <c r="G3" s="28">
         <f t="shared" si="0"/>
         <v>278375.06302774965</v>
       </c>
-      <c r="H3" s="29">
+      <c r="H3" s="28">
         <f t="shared" si="0"/>
         <v>279766.93834288837</v>
       </c>
-      <c r="I3" s="29">
+      <c r="I3" s="28">
         <f t="shared" si="0"/>
         <v>281165.77303460281</v>
       </c>
-      <c r="J3" s="29">
+      <c r="J3" s="28">
         <f t="shared" si="0"/>
         <v>282571.60189977579</v>
       </c>
-      <c r="K3" s="29">
+      <c r="K3" s="28">
         <f t="shared" si="0"/>
         <v>283984.45990927465</v>
       </c>
-      <c r="L3" s="29">
+      <c r="L3" s="28">
         <f t="shared" si="0"/>
         <v>285404.38220882101</v>
       </c>
-      <c r="M3" s="29">
+      <c r="M3" s="28">
         <f t="shared" si="0"/>
         <v>286831.4041198651</v>
       </c>
-      <c r="N3" s="29">
+      <c r="N3" s="28">
         <f t="shared" si="0"/>
         <v>288265.56114046439</v>
       </c>
-      <c r="O3" s="29">
+      <c r="O3" s="28">
         <f t="shared" si="0"/>
         <v>289706.88894616667</v>
       </c>
-      <c r="P3" s="29">
+      <c r="P3" s="28">
         <f t="shared" si="0"/>
         <v>291155.42339089746</v>
       </c>
-      <c r="Q3" s="29">
+      <c r="Q3" s="28">
         <f t="shared" si="0"/>
         <v>292611.2005078519</v>
       </c>
-      <c r="R3" s="29">
+      <c r="R3" s="28">
         <f t="shared" si="0"/>
         <v>294074.25651039113</v>
       </c>
-      <c r="S3" s="29">
+      <c r="S3" s="28">
         <f t="shared" si="0"/>
         <v>295544.62779294304</v>
       </c>
-      <c r="T3" s="29">
+      <c r="T3" s="28">
         <f t="shared" si="0"/>
         <v>297022.35093190771</v>
       </c>
-      <c r="U3" s="29">
+      <c r="U3" s="28">
         <f t="shared" si="0"/>
         <v>298507.46268656722</v>
       </c>
-      <c r="V3" s="29">
+      <c r="V3" s="28">
         <v>300000</v>
       </c>
-      <c r="W3" s="29">
+      <c r="W3" s="28">
         <f t="shared" ref="W3:BB3" si="1">V3*1.005</f>
         <v>301499.99999999994</v>
       </c>
-      <c r="X3" s="29">
+      <c r="X3" s="28">
         <f t="shared" si="1"/>
         <v>303007.49999999988</v>
       </c>
-      <c r="Y3" s="29">
+      <c r="Y3" s="28">
         <f t="shared" si="1"/>
         <v>304522.53749999986</v>
       </c>
-      <c r="Z3" s="29">
+      <c r="Z3" s="28">
         <f t="shared" si="1"/>
         <v>306045.15018749982</v>
       </c>
-      <c r="AA3" s="29">
+      <c r="AA3" s="28">
         <f t="shared" si="1"/>
         <v>307575.3759384373</v>
       </c>
-      <c r="AB3" s="29">
+      <c r="AB3" s="28">
         <f t="shared" si="1"/>
         <v>309113.25281812943</v>
       </c>
-      <c r="AC3" s="29">
+      <c r="AC3" s="28">
         <f t="shared" si="1"/>
         <v>310658.81908222003</v>
       </c>
-      <c r="AD3" s="29">
+      <c r="AD3" s="28">
         <f t="shared" si="1"/>
         <v>312212.11317763111</v>
       </c>
-      <c r="AE3" s="29">
+      <c r="AE3" s="28">
         <f t="shared" si="1"/>
         <v>313773.17374351923</v>
       </c>
-      <c r="AF3" s="29">
+      <c r="AF3" s="28">
         <f t="shared" si="1"/>
         <v>315342.03961223678</v>
       </c>
-      <c r="AG3" s="29">
+      <c r="AG3" s="28">
         <f t="shared" si="1"/>
         <v>316918.74981029792</v>
       </c>
-      <c r="AH3" s="29">
+      <c r="AH3" s="28">
         <f t="shared" si="1"/>
         <v>318503.34355934936</v>
       </c>
-      <c r="AI3" s="29">
+      <c r="AI3" s="28">
         <f t="shared" si="1"/>
         <v>320095.8602771461</v>
       </c>
-      <c r="AJ3" s="29">
+      <c r="AJ3" s="28">
         <f t="shared" si="1"/>
         <v>321696.3395785318</v>
       </c>
-      <c r="AK3" s="29">
+      <c r="AK3" s="28">
         <f t="shared" si="1"/>
         <v>323304.82127642445</v>
       </c>
-      <c r="AL3" s="29">
+      <c r="AL3" s="28">
         <f t="shared" si="1"/>
         <v>324921.34538280655</v>
       </c>
-      <c r="AM3" s="29">
+      <c r="AM3" s="28">
         <f t="shared" si="1"/>
         <v>326545.95210972056</v>
       </c>
-      <c r="AN3" s="29">
+      <c r="AN3" s="28">
         <f t="shared" si="1"/>
         <v>328178.68187026912</v>
       </c>
-      <c r="AO3" s="29">
+      <c r="AO3" s="28">
         <f t="shared" si="1"/>
         <v>329819.57527962042</v>
       </c>
-      <c r="AP3" s="29">
+      <c r="AP3" s="28">
         <f t="shared" si="1"/>
         <v>331468.67315601849</v>
       </c>
-      <c r="AQ3" s="29">
+      <c r="AQ3" s="28">
         <f t="shared" si="1"/>
         <v>333126.01652179856</v>
       </c>
-      <c r="AR3" s="29">
+      <c r="AR3" s="28">
         <f t="shared" si="1"/>
         <v>334791.64660440752</v>
       </c>
-      <c r="AS3" s="29">
+      <c r="AS3" s="28">
         <f t="shared" si="1"/>
         <v>336465.60483742954</v>
       </c>
-      <c r="AT3" s="29">
+      <c r="AT3" s="28">
         <f t="shared" si="1"/>
         <v>338147.93286161666</v>
       </c>
-      <c r="AU3" s="29">
+      <c r="AU3" s="28">
         <f t="shared" si="1"/>
         <v>339838.67252592469</v>
       </c>
-      <c r="AV3" s="29">
+      <c r="AV3" s="28">
         <f t="shared" si="1"/>
         <v>341537.86588855425</v>
       </c>
-      <c r="AW3" s="29">
+      <c r="AW3" s="28">
         <f t="shared" si="1"/>
         <v>343245.555217997</v>
       </c>
-      <c r="AX3" s="29">
+      <c r="AX3" s="28">
         <f t="shared" si="1"/>
         <v>344961.78299408697</v>
       </c>
-      <c r="AY3" s="29">
+      <c r="AY3" s="28">
         <f t="shared" si="1"/>
         <v>346686.59190905734</v>
       </c>
-      <c r="AZ3" s="29">
+      <c r="AZ3" s="28">
         <f t="shared" si="1"/>
         <v>348420.02486860257</v>
       </c>
-      <c r="BA3" s="29">
+      <c r="BA3" s="28">
         <f t="shared" si="1"/>
         <v>350162.12499294552</v>
       </c>
-      <c r="BB3" s="29">
+      <c r="BB3" s="28">
         <f t="shared" si="1"/>
         <v>351912.93561791023</v>
       </c>
-      <c r="BC3" s="29">
+      <c r="BC3" s="28">
         <f t="shared" ref="BC3:CD3" si="2">BB3*1.005</f>
         <v>353672.50029599975</v>
       </c>
-      <c r="BD3" s="29">
+      <c r="BD3" s="28">
         <f t="shared" si="2"/>
         <v>355440.86279747973</v>
       </c>
-      <c r="BE3" s="29">
+      <c r="BE3" s="28">
         <f t="shared" si="2"/>
         <v>357218.06711146707</v>
       </c>
-      <c r="BF3" s="29">
+      <c r="BF3" s="28">
         <f t="shared" si="2"/>
         <v>359004.15744702436</v>
       </c>
-      <c r="BG3" s="29">
+      <c r="BG3" s="28">
         <f t="shared" si="2"/>
         <v>360799.17823425942</v>
       </c>
-      <c r="BH3" s="29">
+      <c r="BH3" s="28">
         <f t="shared" si="2"/>
         <v>362603.1741254307</v>
       </c>
-      <c r="BI3" s="29">
+      <c r="BI3" s="28">
         <f t="shared" si="2"/>
         <v>364416.18999605783</v>
       </c>
-      <c r="BJ3" s="29">
+      <c r="BJ3" s="28">
         <f t="shared" si="2"/>
         <v>366238.27094603807</v>
       </c>
-      <c r="BK3" s="29">
+      <c r="BK3" s="28">
         <f t="shared" si="2"/>
         <v>368069.46230076824</v>
       </c>
-      <c r="BL3" s="29">
+      <c r="BL3" s="28">
         <f t="shared" si="2"/>
         <v>369909.80961227202</v>
       </c>
-      <c r="BM3" s="29">
+      <c r="BM3" s="28">
         <f t="shared" si="2"/>
         <v>371759.35866033332</v>
       </c>
-      <c r="BN3" s="29">
+      <c r="BN3" s="28">
         <f t="shared" si="2"/>
         <v>373618.15545363497</v>
       </c>
-      <c r="BO3" s="29">
+      <c r="BO3" s="28">
         <f t="shared" si="2"/>
         <v>375486.24623090308</v>
       </c>
-      <c r="BP3" s="29">
+      <c r="BP3" s="28">
         <f t="shared" si="2"/>
         <v>377363.67746205756</v>
       </c>
-      <c r="BQ3" s="29">
+      <c r="BQ3" s="28">
         <f t="shared" si="2"/>
         <v>379250.49584936781</v>
       </c>
-      <c r="BR3" s="29">
+      <c r="BR3" s="28">
         <f t="shared" si="2"/>
         <v>381146.74832861463</v>
       </c>
-      <c r="BS3" s="29">
+      <c r="BS3" s="28">
         <f t="shared" si="2"/>
         <v>383052.48207025765</v>
       </c>
-      <c r="BT3" s="29">
+      <c r="BT3" s="28">
         <f t="shared" si="2"/>
         <v>384967.7444806089</v>
       </c>
-      <c r="BU3" s="29">
+      <c r="BU3" s="28">
         <f t="shared" si="2"/>
         <v>386892.58320301189</v>
       </c>
-      <c r="BV3" s="29">
+      <c r="BV3" s="28">
         <f t="shared" si="2"/>
         <v>388827.0461190269</v>
       </c>
-      <c r="BW3" s="29">
+      <c r="BW3" s="28">
         <f t="shared" si="2"/>
         <v>390771.18134962197</v>
       </c>
-      <c r="BX3" s="29">
+      <c r="BX3" s="28">
         <f t="shared" si="2"/>
         <v>392725.03725637007</v>
       </c>
-      <c r="BY3" s="29">
+      <c r="BY3" s="28">
         <f t="shared" si="2"/>
         <v>394688.66244265187</v>
       </c>
-      <c r="BZ3" s="29">
+      <c r="BZ3" s="28">
         <f t="shared" si="2"/>
         <v>396662.1057548651</v>
       </c>
-      <c r="CA3" s="29">
+      <c r="CA3" s="28">
         <f t="shared" si="2"/>
         <v>398645.41628363938</v>
       </c>
-      <c r="CB3" s="29">
+      <c r="CB3" s="28">
         <f t="shared" si="2"/>
         <v>400638.64336505753</v>
       </c>
-      <c r="CC3" s="29">
+      <c r="CC3" s="28">
         <f t="shared" si="2"/>
         <v>402641.83658188279</v>
       </c>
-      <c r="CD3" s="29">
+      <c r="CD3" s="28">
         <f t="shared" si="2"/>
         <v>404655.04576479219</v>
       </c>
     </row>
     <row r="4" spans="1:82" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="29">
+      <c r="B4" s="28">
         <f t="shared" ref="B4:U4" si="3">C4/1.01</f>
         <v>163908.89406745907</v>
       </c>
-      <c r="C4" s="29">
+      <c r="C4" s="28">
         <f t="shared" si="3"/>
         <v>165547.98300813365</v>
       </c>
-      <c r="D4" s="29">
+      <c r="D4" s="28">
         <f t="shared" si="3"/>
         <v>167203.462838215</v>
       </c>
-      <c r="E4" s="29">
+      <c r="E4" s="28">
         <f t="shared" si="3"/>
         <v>168875.49746659715</v>
       </c>
-      <c r="F4" s="29">
+      <c r="F4" s="28">
         <f t="shared" si="3"/>
         <v>170564.25244126312</v>
       </c>
-      <c r="G4" s="29">
+      <c r="G4" s="28">
         <f t="shared" si="3"/>
         <v>172269.89496567575</v>
       </c>
-      <c r="H4" s="29">
+      <c r="H4" s="28">
         <f t="shared" si="3"/>
         <v>173992.59391533252</v>
       </c>
-      <c r="I4" s="29">
+      <c r="I4" s="28">
         <f t="shared" si="3"/>
         <v>175732.51985448584</v>
       </c>
-      <c r="J4" s="29">
+      <c r="J4" s="28">
         <f t="shared" si="3"/>
         <v>177489.8450530307</v>
       </c>
-      <c r="K4" s="29">
+      <c r="K4" s="28">
         <f t="shared" si="3"/>
         <v>179264.74350356101</v>
       </c>
-      <c r="L4" s="29">
+      <c r="L4" s="28">
         <f t="shared" si="3"/>
         <v>181057.39093859663</v>
       </c>
-      <c r="M4" s="29">
+      <c r="M4" s="28">
         <f t="shared" si="3"/>
         <v>182867.9648479826</v>
       </c>
-      <c r="N4" s="29">
+      <c r="N4" s="28">
         <f t="shared" si="3"/>
         <v>184696.64449646242</v>
       </c>
-      <c r="O4" s="29">
+      <c r="O4" s="28">
         <f t="shared" si="3"/>
         <v>186543.61094142706</v>
       </c>
-      <c r="P4" s="29">
+      <c r="P4" s="28">
         <f t="shared" si="3"/>
         <v>188409.04705084133</v>
       </c>
-      <c r="Q4" s="29">
+      <c r="Q4" s="28">
         <f t="shared" si="3"/>
         <v>190293.13752134974</v>
       </c>
-      <c r="R4" s="29">
+      <c r="R4" s="28">
         <f t="shared" si="3"/>
         <v>192196.06889656323</v>
       </c>
-      <c r="S4" s="29">
+      <c r="S4" s="28">
         <f t="shared" si="3"/>
         <v>194118.02958552886</v>
       </c>
-      <c r="T4" s="29">
+      <c r="T4" s="28">
         <f t="shared" si="3"/>
         <v>196059.20988138416</v>
       </c>
-      <c r="U4" s="29">
+      <c r="U4" s="28">
         <f t="shared" si="3"/>
         <v>198019.80198019801</v>
       </c>
-      <c r="V4" s="29">
+      <c r="V4" s="28">
         <v>200000</v>
       </c>
-      <c r="W4" s="29">
+      <c r="W4" s="28">
         <f>V4*1.01</f>
         <v>202000</v>
       </c>
-      <c r="X4" s="29">
+      <c r="X4" s="28">
         <f>W4*1.01</f>
         <v>204020</v>
       </c>
-      <c r="Y4" s="29">
+      <c r="Y4" s="28">
         <f>X4*1.01</f>
         <v>206060.2</v>
       </c>
-      <c r="Z4" s="29">
+      <c r="Z4" s="28">
         <f>Y4*1.01</f>
         <v>208120.80200000003</v>
       </c>
-      <c r="AA4" s="29">
+      <c r="AA4" s="28">
         <f t="shared" ref="AA4:CD4" si="4">Z4*1.01</f>
         <v>210202.01002000002</v>
       </c>
-      <c r="AB4" s="29">
+      <c r="AB4" s="28">
         <f t="shared" si="4"/>
         <v>212304.03012020001</v>
       </c>
-      <c r="AC4" s="29">
+      <c r="AC4" s="28">
         <f t="shared" si="4"/>
         <v>214427.07042140202</v>
       </c>
-      <c r="AD4" s="29">
+      <c r="AD4" s="28">
         <f t="shared" si="4"/>
         <v>216571.34112561605</v>
       </c>
-      <c r="AE4" s="29">
+      <c r="AE4" s="28">
         <f t="shared" si="4"/>
         <v>218737.05453687222</v>
       </c>
-      <c r="AF4" s="29">
+      <c r="AF4" s="28">
         <f t="shared" si="4"/>
         <v>220924.42508224095</v>
       </c>
-      <c r="AG4" s="29">
+      <c r="AG4" s="28">
         <f t="shared" si="4"/>
         <v>223133.66933306336</v>
       </c>
-      <c r="AH4" s="29">
+      <c r="AH4" s="28">
         <f t="shared" si="4"/>
         <v>225365.006026394</v>
       </c>
-      <c r="AI4" s="29">
+      <c r="AI4" s="28">
         <f t="shared" si="4"/>
         <v>227618.65608665792</v>
       </c>
-      <c r="AJ4" s="29">
+      <c r="AJ4" s="28">
         <f t="shared" si="4"/>
         <v>229894.84264752449</v>
       </c>
-      <c r="AK4" s="29">
+      <c r="AK4" s="28">
         <f t="shared" si="4"/>
         <v>232193.79107399975</v>
       </c>
-      <c r="AL4" s="29">
+      <c r="AL4" s="28">
         <f t="shared" si="4"/>
         <v>234515.72898473975</v>
       </c>
-      <c r="AM4" s="29">
+      <c r="AM4" s="28">
         <f t="shared" si="4"/>
         <v>236860.88627458716</v>
       </c>
-      <c r="AN4" s="29">
+      <c r="AN4" s="28">
         <f t="shared" si="4"/>
         <v>239229.49513733303</v>
       </c>
-      <c r="AO4" s="29">
+      <c r="AO4" s="28">
         <f t="shared" si="4"/>
         <v>241621.79008870636</v>
       </c>
-      <c r="AP4" s="29">
+      <c r="AP4" s="28">
         <f t="shared" si="4"/>
         <v>244038.00798959343</v>
       </c>
-      <c r="AQ4" s="29">
+      <c r="AQ4" s="28">
         <f t="shared" si="4"/>
         <v>246478.38806948936</v>
       </c>
-      <c r="AR4" s="29">
+      <c r="AR4" s="28">
         <f t="shared" si="4"/>
         <v>248943.17195018425</v>
       </c>
-      <c r="AS4" s="29">
+      <c r="AS4" s="28">
         <f t="shared" si="4"/>
         <v>251432.6036696861</v>
       </c>
-      <c r="AT4" s="29">
+      <c r="AT4" s="28">
         <f t="shared" si="4"/>
         <v>253946.92970638297</v>
       </c>
-      <c r="AU4" s="29">
+      <c r="AU4" s="28">
         <f t="shared" si="4"/>
         <v>256486.3990034468</v>
       </c>
-      <c r="AV4" s="29">
+      <c r="AV4" s="28">
         <f t="shared" si="4"/>
         <v>259051.26299348127</v>
       </c>
-      <c r="AW4" s="29">
+      <c r="AW4" s="28">
         <f t="shared" si="4"/>
         <v>261641.77562341609</v>
       </c>
-      <c r="AX4" s="29">
+      <c r="AX4" s="28">
         <f t="shared" si="4"/>
         <v>264258.19337965024</v>
       </c>
-      <c r="AY4" s="29">
+      <c r="AY4" s="28">
         <f t="shared" si="4"/>
         <v>266900.77531344676</v>
       </c>
-      <c r="AZ4" s="29">
+      <c r="AZ4" s="28">
         <f t="shared" si="4"/>
         <v>269569.78306658124</v>
       </c>
-      <c r="BA4" s="29">
+      <c r="BA4" s="28">
         <f t="shared" si="4"/>
         <v>272265.48089724703</v>
       </c>
-      <c r="BB4" s="29">
+      <c r="BB4" s="28">
         <f t="shared" si="4"/>
         <v>274988.13570621953</v>
       </c>
-      <c r="BC4" s="29">
+      <c r="BC4" s="28">
         <f t="shared" si="4"/>
         <v>277738.01706328173</v>
       </c>
-      <c r="BD4" s="29">
+      <c r="BD4" s="28">
         <f t="shared" si="4"/>
         <v>280515.39723391453</v>
       </c>
-      <c r="BE4" s="29">
+      <c r="BE4" s="28">
         <f t="shared" si="4"/>
         <v>283320.5512062537</v>
       </c>
-      <c r="BF4" s="29">
+      <c r="BF4" s="28">
         <f t="shared" si="4"/>
         <v>286153.75671831623</v>
       </c>
-      <c r="BG4" s="29">
+      <c r="BG4" s="28">
         <f t="shared" si="4"/>
         <v>289015.29428549937</v>
       </c>
-      <c r="BH4" s="29">
+      <c r="BH4" s="28">
         <f t="shared" si="4"/>
         <v>291905.44722835434</v>
       </c>
-      <c r="BI4" s="29">
+      <c r="BI4" s="28">
         <f t="shared" si="4"/>
         <v>294824.50170063786</v>
       </c>
-      <c r="BJ4" s="29">
+      <c r="BJ4" s="28">
         <f t="shared" si="4"/>
         <v>297772.74671764422</v>
       </c>
-      <c r="BK4" s="29">
+      <c r="BK4" s="28">
         <f t="shared" si="4"/>
         <v>300750.47418482066</v>
       </c>
-      <c r="BL4" s="29">
+      <c r="BL4" s="28">
         <f t="shared" si="4"/>
         <v>303757.97892666887</v>
       </c>
-      <c r="BM4" s="29">
+      <c r="BM4" s="28">
         <f t="shared" si="4"/>
         <v>306795.55871593556</v>
       </c>
-      <c r="BN4" s="29">
+      <c r="BN4" s="28">
         <f t="shared" si="4"/>
         <v>309863.51430309494</v>
       </c>
-      <c r="BO4" s="29">
+      <c r="BO4" s="28">
         <f t="shared" si="4"/>
         <v>312962.1494461259</v>
       </c>
-      <c r="BP4" s="29">
+      <c r="BP4" s="28">
         <f t="shared" si="4"/>
         <v>316091.77094058716</v>
       </c>
-      <c r="BQ4" s="29">
+      <c r="BQ4" s="28">
         <f t="shared" si="4"/>
         <v>319252.68864999304</v>
       </c>
-      <c r="BR4" s="29">
+      <c r="BR4" s="28">
         <f t="shared" si="4"/>
         <v>322445.21553649299</v>
       </c>
-      <c r="BS4" s="29">
+      <c r="BS4" s="28">
         <f t="shared" si="4"/>
         <v>325669.6676918579</v>
       </c>
-      <c r="BT4" s="29">
+      <c r="BT4" s="28">
         <f t="shared" si="4"/>
         <v>328926.3643687765</v>
       </c>
-      <c r="BU4" s="29">
+      <c r="BU4" s="28">
         <f t="shared" si="4"/>
         <v>332215.62801246427</v>
       </c>
-      <c r="BV4" s="29">
+      <c r="BV4" s="28">
         <f t="shared" si="4"/>
         <v>335537.78429258888</v>
       </c>
-      <c r="BW4" s="29">
+      <c r="BW4" s="28">
         <f t="shared" si="4"/>
         <v>338893.16213551478</v>
       </c>
-      <c r="BX4" s="29">
+      <c r="BX4" s="28">
         <f t="shared" si="4"/>
         <v>342282.09375686996</v>
       </c>
-      <c r="BY4" s="29">
+      <c r="BY4" s="28">
         <f t="shared" si="4"/>
         <v>345704.91469443869</v>
       </c>
-      <c r="BZ4" s="29">
+      <c r="BZ4" s="28">
         <f t="shared" si="4"/>
         <v>349161.96384138305</v>
       </c>
-      <c r="CA4" s="29">
+      <c r="CA4" s="28">
         <f t="shared" si="4"/>
         <v>352653.58347979689</v>
       </c>
-      <c r="CB4" s="29">
+      <c r="CB4" s="28">
         <f t="shared" si="4"/>
         <v>356180.11931459483</v>
       </c>
-      <c r="CC4" s="29">
+      <c r="CC4" s="28">
         <f t="shared" si="4"/>
         <v>359741.92050774081</v>
       </c>
-      <c r="CD4" s="29">
+      <c r="CD4" s="28">
         <f t="shared" si="4"/>
         <v>363339.33971281821</v>
       </c>
@@ -3915,6 +4481,165 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0149604-0477-4296-92AB-E87FF5ABA3A8}">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:B84"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="16" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11"/>
+      <c r="B1" s="13"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="8"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="8">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="15"/>
+      <c r="B55" s="9"/>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="15"/>
+      <c r="B56" s="9"/>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="15"/>
+      <c r="B57" s="9"/>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="15"/>
+      <c r="B58" s="9"/>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="15"/>
+      <c r="B59" s="9"/>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="15"/>
+      <c r="B60" s="9"/>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="15"/>
+      <c r="B61" s="9"/>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="15"/>
+      <c r="B62" s="9"/>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="15"/>
+      <c r="B63" s="9"/>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="15"/>
+      <c r="B64" s="9"/>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="15"/>
+      <c r="B65" s="9"/>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="15"/>
+      <c r="B66" s="9"/>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="15"/>
+      <c r="B67" s="9"/>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="15"/>
+      <c r="B68" s="9"/>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="15"/>
+      <c r="B69" s="9"/>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="15"/>
+      <c r="B70" s="9"/>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="15"/>
+      <c r="B71" s="9"/>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="15"/>
+      <c r="B72" s="9"/>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="15"/>
+      <c r="B73" s="9"/>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="15"/>
+      <c r="B74" s="9"/>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="15"/>
+      <c r="B75" s="9"/>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="15"/>
+      <c r="B76" s="9"/>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="15"/>
+      <c r="B77" s="9"/>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="15"/>
+      <c r="B78" s="9"/>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="15"/>
+      <c r="B79" s="9"/>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="15"/>
+      <c r="B80" s="9"/>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="15"/>
+      <c r="B81" s="9"/>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="15"/>
+      <c r="B82" s="9"/>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="15"/>
+      <c r="B83" s="9"/>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="15"/>
+      <c r="B84" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
@@ -4073,7 +4798,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
@@ -4089,7 +4814,7 @@
     <col min="1" max="1" width="9.140625" style="26" customWidth="1"/>
     <col min="2" max="2" width="12.140625" style="25" customWidth="1"/>
     <col min="3" max="5" width="11" style="1" hidden="1" customWidth="1"/>
-    <col min="6" max="7" width="11" style="35" hidden="1" customWidth="1"/>
+    <col min="6" max="7" width="11" style="34" hidden="1" customWidth="1"/>
     <col min="8" max="22" width="11" style="1" hidden="1" customWidth="1"/>
     <col min="23" max="76" width="11" style="1" customWidth="1"/>
     <col min="77" max="83" width="9.42578125" style="16" bestFit="1" customWidth="1"/>
@@ -4100,80 +4825,80 @@
         <v>46</v>
       </c>
       <c r="B1" s="12"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="34"/>
-      <c r="V1" s="34"/>
-      <c r="W1" s="34"/>
-      <c r="X1" s="34"/>
-      <c r="Y1" s="34"/>
-      <c r="Z1" s="34"/>
-      <c r="AA1" s="34"/>
-      <c r="AB1" s="34"/>
-      <c r="AC1" s="34"/>
-      <c r="AD1" s="34"/>
-      <c r="AE1" s="34"/>
-      <c r="AF1" s="34"/>
-      <c r="AG1" s="34"/>
-      <c r="AH1" s="34"/>
-      <c r="AI1" s="34"/>
-      <c r="AJ1" s="34"/>
-      <c r="AK1" s="34"/>
-      <c r="AL1" s="34"/>
-      <c r="AM1" s="34"/>
-      <c r="AN1" s="34"/>
-      <c r="AO1" s="34"/>
-      <c r="AP1" s="34"/>
-      <c r="AQ1" s="34"/>
-      <c r="AR1" s="34"/>
-      <c r="AS1" s="34"/>
-      <c r="AT1" s="34"/>
-      <c r="AU1" s="34"/>
-      <c r="AV1" s="34"/>
-      <c r="AW1" s="34"/>
-      <c r="AX1" s="34"/>
-      <c r="AY1" s="34"/>
-      <c r="AZ1" s="34"/>
-      <c r="BA1" s="34"/>
-      <c r="BB1" s="34"/>
-      <c r="BC1" s="34"/>
-      <c r="BD1" s="34"/>
-      <c r="BE1" s="34"/>
-      <c r="BF1" s="34"/>
-      <c r="BG1" s="34"/>
-      <c r="BH1" s="34"/>
-      <c r="BI1" s="34"/>
-      <c r="BJ1" s="34"/>
-      <c r="BK1" s="34"/>
-      <c r="BL1" s="34"/>
-      <c r="BM1" s="34"/>
-      <c r="BN1" s="34"/>
-      <c r="BO1" s="34"/>
-      <c r="BP1" s="34"/>
-      <c r="BQ1" s="34"/>
-      <c r="BR1" s="34"/>
-      <c r="BS1" s="34"/>
-      <c r="BT1" s="34"/>
-      <c r="BU1" s="34"/>
-      <c r="BV1" s="34"/>
-      <c r="BW1" s="34"/>
-      <c r="BX1" s="34"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
+      <c r="U1" s="33"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="33"/>
+      <c r="X1" s="33"/>
+      <c r="Y1" s="33"/>
+      <c r="Z1" s="33"/>
+      <c r="AA1" s="33"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="33"/>
+      <c r="AD1" s="33"/>
+      <c r="AE1" s="33"/>
+      <c r="AF1" s="33"/>
+      <c r="AG1" s="33"/>
+      <c r="AH1" s="33"/>
+      <c r="AI1" s="33"/>
+      <c r="AJ1" s="33"/>
+      <c r="AK1" s="33"/>
+      <c r="AL1" s="33"/>
+      <c r="AM1" s="33"/>
+      <c r="AN1" s="33"/>
+      <c r="AO1" s="33"/>
+      <c r="AP1" s="33"/>
+      <c r="AQ1" s="33"/>
+      <c r="AR1" s="33"/>
+      <c r="AS1" s="33"/>
+      <c r="AT1" s="33"/>
+      <c r="AU1" s="33"/>
+      <c r="AV1" s="33"/>
+      <c r="AW1" s="33"/>
+      <c r="AX1" s="33"/>
+      <c r="AY1" s="33"/>
+      <c r="AZ1" s="33"/>
+      <c r="BA1" s="33"/>
+      <c r="BB1" s="33"/>
+      <c r="BC1" s="33"/>
+      <c r="BD1" s="33"/>
+      <c r="BE1" s="33"/>
+      <c r="BF1" s="33"/>
+      <c r="BG1" s="33"/>
+      <c r="BH1" s="33"/>
+      <c r="BI1" s="33"/>
+      <c r="BJ1" s="33"/>
+      <c r="BK1" s="33"/>
+      <c r="BL1" s="33"/>
+      <c r="BM1" s="33"/>
+      <c r="BN1" s="33"/>
+      <c r="BO1" s="33"/>
+      <c r="BP1" s="33"/>
+      <c r="BQ1" s="33"/>
+      <c r="BR1" s="33"/>
+      <c r="BS1" s="33"/>
+      <c r="BT1" s="33"/>
+      <c r="BU1" s="33"/>
+      <c r="BV1" s="33"/>
+      <c r="BW1" s="33"/>
+      <c r="BX1" s="33"/>
     </row>
     <row r="2" spans="1:83" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
@@ -5353,326 +6078,326 @@
       <c r="B6" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="36">
+      <c r="C6" s="35">
         <v>8</v>
       </c>
-      <c r="D6" s="36">
+      <c r="D6" s="35">
         <v>8</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="35">
         <v>8</v>
       </c>
-      <c r="F6" s="36">
+      <c r="F6" s="35">
         <v>8</v>
       </c>
-      <c r="G6" s="36">
+      <c r="G6" s="35">
         <v>8</v>
       </c>
-      <c r="H6" s="36">
+      <c r="H6" s="35">
         <v>8</v>
       </c>
-      <c r="I6" s="36">
+      <c r="I6" s="35">
         <v>8</v>
       </c>
-      <c r="J6" s="36">
+      <c r="J6" s="35">
         <v>8</v>
       </c>
-      <c r="K6" s="36">
+      <c r="K6" s="35">
         <v>8</v>
       </c>
-      <c r="L6" s="36">
+      <c r="L6" s="35">
         <v>8</v>
       </c>
-      <c r="M6" s="36">
+      <c r="M6" s="35">
         <v>8</v>
       </c>
-      <c r="N6" s="36">
+      <c r="N6" s="35">
         <v>8</v>
       </c>
-      <c r="O6" s="36">
+      <c r="O6" s="35">
         <v>8</v>
       </c>
-      <c r="P6" s="36">
+      <c r="P6" s="35">
         <v>8</v>
       </c>
-      <c r="Q6" s="36">
+      <c r="Q6" s="35">
         <v>8</v>
       </c>
-      <c r="R6" s="36">
+      <c r="R6" s="35">
         <v>8</v>
       </c>
-      <c r="S6" s="36">
+      <c r="S6" s="35">
         <v>8</v>
       </c>
-      <c r="T6" s="36">
+      <c r="T6" s="35">
         <v>8</v>
       </c>
-      <c r="U6" s="36">
+      <c r="U6" s="35">
         <v>8</v>
       </c>
-      <c r="V6" s="36">
+      <c r="V6" s="35">
         <v>8</v>
       </c>
-      <c r="W6" s="36">
+      <c r="W6" s="35">
         <v>8</v>
       </c>
-      <c r="X6" s="36">
+      <c r="X6" s="35">
         <v>8</v>
       </c>
-      <c r="Y6" s="36">
+      <c r="Y6" s="35">
         <v>8</v>
       </c>
-      <c r="Z6" s="36">
+      <c r="Z6" s="35">
         <v>8</v>
       </c>
-      <c r="AA6" s="36">
+      <c r="AA6" s="35">
         <v>8</v>
       </c>
-      <c r="AB6" s="36">
+      <c r="AB6" s="35">
         <f>AA6*1.004</f>
         <v>8.032</v>
       </c>
-      <c r="AC6" s="36">
+      <c r="AC6" s="35">
         <f>AB6*1.025</f>
         <v>8.2327999999999992</v>
       </c>
-      <c r="AD6" s="36">
+      <c r="AD6" s="35">
         <f t="shared" ref="AD6:AQ6" si="9">AC6*1.025</f>
         <v>8.4386199999999985</v>
       </c>
-      <c r="AE6" s="36">
+      <c r="AE6" s="35">
         <f t="shared" si="9"/>
         <v>8.649585499999997</v>
       </c>
-      <c r="AF6" s="36">
+      <c r="AF6" s="35">
         <f t="shared" si="9"/>
         <v>8.8658251374999963</v>
       </c>
-      <c r="AG6" s="36">
+      <c r="AG6" s="35">
         <f t="shared" si="9"/>
         <v>9.0874707659374963</v>
       </c>
-      <c r="AH6" s="36">
+      <c r="AH6" s="35">
         <f t="shared" si="9"/>
         <v>9.3146575350859333</v>
       </c>
-      <c r="AI6" s="36">
+      <c r="AI6" s="35">
         <f t="shared" si="9"/>
         <v>9.5475239734630808</v>
       </c>
-      <c r="AJ6" s="36">
+      <c r="AJ6" s="35">
         <f t="shared" si="9"/>
         <v>9.7862120727996569</v>
       </c>
-      <c r="AK6" s="36">
+      <c r="AK6" s="35">
         <f t="shared" si="9"/>
         <v>10.030867374619648</v>
       </c>
-      <c r="AL6" s="36">
+      <c r="AL6" s="35">
         <f t="shared" si="9"/>
         <v>10.281639058985139</v>
       </c>
-      <c r="AM6" s="36">
+      <c r="AM6" s="35">
         <f t="shared" si="9"/>
         <v>10.538680035459766</v>
       </c>
-      <c r="AN6" s="36">
+      <c r="AN6" s="35">
         <f t="shared" si="9"/>
         <v>10.802147036346259</v>
       </c>
-      <c r="AO6" s="36">
+      <c r="AO6" s="35">
         <f t="shared" si="9"/>
         <v>11.072200712254915</v>
       </c>
-      <c r="AP6" s="36">
+      <c r="AP6" s="35">
         <f t="shared" si="9"/>
         <v>11.349005730061286</v>
       </c>
-      <c r="AQ6" s="36">
+      <c r="AQ6" s="35">
         <f t="shared" si="9"/>
         <v>11.632730873312818</v>
       </c>
-      <c r="AR6" s="36">
+      <c r="AR6" s="35">
         <f>AQ6*0.983</f>
         <v>11.4349744484665</v>
       </c>
-      <c r="AS6" s="36">
+      <c r="AS6" s="35">
         <f t="shared" ref="AS6:CC6" si="10">AR6*0.983</f>
         <v>11.240579882842569</v>
       </c>
-      <c r="AT6" s="36">
+      <c r="AT6" s="35">
         <f t="shared" si="10"/>
         <v>11.049490024834245</v>
       </c>
-      <c r="AU6" s="36">
+      <c r="AU6" s="35">
         <f t="shared" si="10"/>
         <v>10.861648694412063</v>
       </c>
-      <c r="AV6" s="36">
+      <c r="AV6" s="35">
         <f t="shared" si="10"/>
         <v>10.677000666607057</v>
       </c>
-      <c r="AW6" s="36">
+      <c r="AW6" s="35">
         <f t="shared" si="10"/>
         <v>10.495491655274737</v>
       </c>
-      <c r="AX6" s="36">
+      <c r="AX6" s="35">
         <f t="shared" si="10"/>
         <v>10.317068297135066</v>
       </c>
-      <c r="AY6" s="36">
+      <c r="AY6" s="35">
         <f t="shared" si="10"/>
         <v>10.141678136083769</v>
       </c>
-      <c r="AZ6" s="36">
+      <c r="AZ6" s="35">
         <f t="shared" si="10"/>
         <v>9.9692696077703449</v>
       </c>
-      <c r="BA6" s="36">
+      <c r="BA6" s="35">
         <f t="shared" si="10"/>
         <v>9.7997920244382488</v>
       </c>
-      <c r="BB6" s="36">
+      <c r="BB6" s="35">
         <f t="shared" si="10"/>
         <v>9.6331955600227985</v>
       </c>
-      <c r="BC6" s="36">
+      <c r="BC6" s="35">
         <f t="shared" si="10"/>
         <v>9.4694312355024106</v>
       </c>
-      <c r="BD6" s="36">
+      <c r="BD6" s="35">
         <f t="shared" si="10"/>
         <v>9.3084509044988692</v>
       </c>
-      <c r="BE6" s="36">
+      <c r="BE6" s="35">
         <f t="shared" si="10"/>
         <v>9.1502072391223876</v>
       </c>
-      <c r="BF6" s="36">
+      <c r="BF6" s="35">
         <f t="shared" si="10"/>
         <v>8.9946537160573072</v>
       </c>
-      <c r="BG6" s="36">
+      <c r="BG6" s="35">
         <f t="shared" si="10"/>
         <v>8.8417446028843329</v>
       </c>
-      <c r="BH6" s="36">
+      <c r="BH6" s="35">
         <f t="shared" si="10"/>
         <v>8.691434944635299</v>
       </c>
-      <c r="BI6" s="36">
+      <c r="BI6" s="35">
         <f t="shared" si="10"/>
         <v>8.5436805505764983</v>
       </c>
-      <c r="BJ6" s="36">
+      <c r="BJ6" s="35">
         <f t="shared" si="10"/>
         <v>8.3984379812166985</v>
       </c>
-      <c r="BK6" s="36">
+      <c r="BK6" s="35">
         <f t="shared" si="10"/>
         <v>8.255664535536015</v>
       </c>
-      <c r="BL6" s="36">
+      <c r="BL6" s="35">
         <f t="shared" si="10"/>
         <v>8.115318238431902</v>
       </c>
-      <c r="BM6" s="36">
+      <c r="BM6" s="35">
         <f t="shared" si="10"/>
         <v>7.97735782837856</v>
       </c>
-      <c r="BN6" s="36">
+      <c r="BN6" s="35">
         <f t="shared" si="10"/>
         <v>7.8417427452961244</v>
       </c>
-      <c r="BO6" s="36">
+      <c r="BO6" s="35">
         <f t="shared" si="10"/>
         <v>7.7084331186260897</v>
       </c>
-      <c r="BP6" s="36">
+      <c r="BP6" s="35">
         <f t="shared" si="10"/>
         <v>7.5773897556094463</v>
       </c>
-      <c r="BQ6" s="36">
+      <c r="BQ6" s="35">
         <f t="shared" si="10"/>
         <v>7.4485741297640855</v>
       </c>
-      <c r="BR6" s="36">
+      <c r="BR6" s="35">
         <f t="shared" si="10"/>
         <v>7.321948369558096</v>
       </c>
-      <c r="BS6" s="36">
+      <c r="BS6" s="35">
         <f t="shared" si="10"/>
         <v>7.1974752472756087</v>
       </c>
-      <c r="BT6" s="36">
+      <c r="BT6" s="35">
         <f t="shared" si="10"/>
         <v>7.0751181680719233</v>
       </c>
-      <c r="BU6" s="36">
+      <c r="BU6" s="35">
         <f t="shared" si="10"/>
         <v>6.9548411592147001</v>
       </c>
-      <c r="BV6" s="36">
+      <c r="BV6" s="35">
         <f t="shared" si="10"/>
         <v>6.8366088595080505</v>
       </c>
-      <c r="BW6" s="36">
+      <c r="BW6" s="35">
         <f t="shared" si="10"/>
         <v>6.7203865088964134</v>
       </c>
-      <c r="BX6" s="36">
+      <c r="BX6" s="35">
         <f t="shared" si="10"/>
         <v>6.6061399382451746</v>
       </c>
-      <c r="BY6" s="36">
+      <c r="BY6" s="35">
         <f t="shared" si="10"/>
         <v>6.4938355592950066</v>
       </c>
-      <c r="BZ6" s="36">
+      <c r="BZ6" s="35">
         <f t="shared" si="10"/>
         <v>6.3834403547869911</v>
       </c>
-      <c r="CA6" s="36">
+      <c r="CA6" s="35">
         <f t="shared" si="10"/>
         <v>6.2749218687556123</v>
       </c>
-      <c r="CB6" s="36">
+      <c r="CB6" s="35">
         <f t="shared" si="10"/>
         <v>6.1682481969867666</v>
       </c>
-      <c r="CC6" s="36">
+      <c r="CC6" s="35">
         <f t="shared" si="10"/>
         <v>6.0633879776379915</v>
       </c>
-      <c r="CD6" s="36">
+      <c r="CD6" s="35">
         <f t="shared" ref="CD6:CE6" si="11">CC6*1.001</f>
         <v>6.0694513656156293</v>
       </c>
-      <c r="CE6" s="36">
+      <c r="CE6" s="35">
         <f t="shared" si="11"/>
         <v>6.0755208169812445</v>
       </c>
     </row>
     <row r="7" spans="1:83" x14ac:dyDescent="0.25">
       <c r="B7" s="27"/>
-      <c r="C7" s="35"/>
+      <c r="C7" s="34"/>
     </row>
     <row r="8" spans="1:83" x14ac:dyDescent="0.25">
       <c r="B8" s="27"/>
-      <c r="C8" s="35"/>
+      <c r="C8" s="34"/>
     </row>
     <row r="9" spans="1:83" x14ac:dyDescent="0.25">
       <c r="B9" s="27"/>
-      <c r="C9" s="35"/>
+      <c r="C9" s="34"/>
     </row>
     <row r="10" spans="1:83" x14ac:dyDescent="0.25">
       <c r="B10" s="27"/>
-      <c r="C10" s="35"/>
+      <c r="C10" s="34"/>
     </row>
     <row r="11" spans="1:83" x14ac:dyDescent="0.25">
       <c r="B11" s="27"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5680,7 +6405,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
@@ -6761,15 +7486,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:CF6"/>
   <sheetViews>
-    <sheetView topLeftCell="BN1" workbookViewId="0">
-      <selection activeCell="P31" sqref="P31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8363,473 +9088,4 @@
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <sheetPr>
-    <tabColor rgb="FFFFFF00"/>
-  </sheetPr>
-  <dimension ref="A1:J21"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.7109375" style="16" customWidth="1"/>
-    <col min="2" max="2" width="15" style="16" customWidth="1"/>
-    <col min="3" max="3" width="12" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14" style="16" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" s="14" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2"/>
-      <c r="J2" s="16"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="51" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="37">
-        <v>17.600000000000001</v>
-      </c>
-      <c r="C3" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3" s="18">
-        <v>2197</v>
-      </c>
-      <c r="E3" s="19">
-        <v>1.88</v>
-      </c>
-      <c r="F3" s="53">
-        <v>188.72813508993531</v>
-      </c>
-      <c r="I3"/>
-      <c r="J3" s="16"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="51" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="37">
-        <v>26.6</v>
-      </c>
-      <c r="C4" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="D4" s="21">
-        <v>2795</v>
-      </c>
-      <c r="E4">
-        <v>2.41</v>
-      </c>
-      <c r="F4" s="54">
-        <v>259.37886848165812</v>
-      </c>
-      <c r="H4" s="16"/>
-      <c r="J4" s="16"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="51" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="37">
-        <v>42.2</v>
-      </c>
-      <c r="C5" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="D5" s="21">
-        <v>4106</v>
-      </c>
-      <c r="E5">
-        <v>3.86</v>
-      </c>
-      <c r="F5" s="54">
-        <v>379.61240300552259</v>
-      </c>
-      <c r="H5" s="16"/>
-      <c r="J5" s="16"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="51" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="37">
-        <v>26.6</v>
-      </c>
-      <c r="C6" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="21">
-        <v>2795</v>
-      </c>
-      <c r="E6">
-        <v>2.41</v>
-      </c>
-      <c r="F6" s="54">
-        <v>259.37886848165812</v>
-      </c>
-      <c r="H6" s="16"/>
-      <c r="J6" s="16"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="51" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="37">
-        <v>42.2</v>
-      </c>
-      <c r="C7" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" s="21">
-        <v>4106</v>
-      </c>
-      <c r="E7">
-        <v>3.86</v>
-      </c>
-      <c r="F7" s="54">
-        <v>379.61240300552259</v>
-      </c>
-      <c r="H7" s="16"/>
-      <c r="J7" s="16"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="51" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="37">
-        <v>26.6</v>
-      </c>
-      <c r="C8" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="D8" s="21">
-        <v>2795</v>
-      </c>
-      <c r="E8">
-        <v>2.41</v>
-      </c>
-      <c r="F8" s="54">
-        <v>259.37886848165812</v>
-      </c>
-      <c r="H8" s="16"/>
-      <c r="J8" s="16"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="51" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="37">
-        <v>42.2</v>
-      </c>
-      <c r="C9" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="21">
-        <v>4106</v>
-      </c>
-      <c r="E9">
-        <v>3.86</v>
-      </c>
-      <c r="F9" s="54">
-        <v>379.61240300552259</v>
-      </c>
-      <c r="H9" s="16"/>
-      <c r="J9" s="16"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="51" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="37">
-        <v>59.9</v>
-      </c>
-      <c r="C10" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" s="21">
-        <v>7000</v>
-      </c>
-      <c r="E10">
-        <v>5.17</v>
-      </c>
-      <c r="F10" s="54">
-        <v>506.94546978896818</v>
-      </c>
-      <c r="H10" s="16"/>
-      <c r="J10" s="16"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="51" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="37">
-        <v>59.9</v>
-      </c>
-      <c r="C11" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="21">
-        <v>7000</v>
-      </c>
-      <c r="E11">
-        <v>5.17</v>
-      </c>
-      <c r="F11" s="54">
-        <v>506.94546978896818</v>
-      </c>
-      <c r="H11" s="16"/>
-      <c r="J11" s="16"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="51" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="37">
-        <v>75</v>
-      </c>
-      <c r="C12" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="D12" s="21">
-        <v>8191</v>
-      </c>
-      <c r="E12">
-        <v>6.95</v>
-      </c>
-      <c r="F12" s="54">
-        <v>684.27360431283273</v>
-      </c>
-      <c r="H12" s="16"/>
-      <c r="J12" s="16"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="51" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="37">
-        <v>75</v>
-      </c>
-      <c r="C13" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" s="21">
-        <v>8191</v>
-      </c>
-      <c r="E13">
-        <v>6.95</v>
-      </c>
-      <c r="F13" s="54">
-        <v>684.27360431283273</v>
-      </c>
-      <c r="H13" s="16"/>
-      <c r="J13" s="16"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="51" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="37">
-        <v>89.8</v>
-      </c>
-      <c r="C14" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="D14" s="21">
-        <v>11900</v>
-      </c>
-      <c r="E14">
-        <v>7.63</v>
-      </c>
-      <c r="F14" s="54">
-        <v>740.03953883669703</v>
-      </c>
-      <c r="H14" s="16"/>
-      <c r="J14" s="16"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="51" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="37">
-        <v>95</v>
-      </c>
-      <c r="C15" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" s="21">
-        <v>12453</v>
-      </c>
-      <c r="E15">
-        <v>7.87</v>
-      </c>
-      <c r="F15" s="54">
-        <v>856.08018367798525</v>
-      </c>
-      <c r="H15" s="16"/>
-      <c r="J15" s="16"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="51" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="37">
-        <v>100</v>
-      </c>
-      <c r="C16" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="D16" s="21">
-        <v>13566</v>
-      </c>
-      <c r="E16">
-        <v>8.4499999999999993</v>
-      </c>
-      <c r="F16" s="54">
-        <v>837.373293546117</v>
-      </c>
-      <c r="H16" s="16"/>
-      <c r="J16" s="16"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="51" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="37">
-        <v>89.8</v>
-      </c>
-      <c r="C17" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" s="21">
-        <v>11900</v>
-      </c>
-      <c r="E17">
-        <v>7.63</v>
-      </c>
-      <c r="F17" s="54">
-        <v>740.03953883669703</v>
-      </c>
-      <c r="H17" s="16"/>
-      <c r="J17" s="16"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="51" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" s="37">
-        <v>95</v>
-      </c>
-      <c r="C18" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" s="21">
-        <v>12453</v>
-      </c>
-      <c r="E18">
-        <v>7.87</v>
-      </c>
-      <c r="F18" s="54">
-        <v>856.08018367798525</v>
-      </c>
-      <c r="H18" s="16"/>
-      <c r="J18" s="28"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="51" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="37">
-        <v>100</v>
-      </c>
-      <c r="C19" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="D19" s="21">
-        <v>13566</v>
-      </c>
-      <c r="E19">
-        <v>8.4499999999999993</v>
-      </c>
-      <c r="F19" s="54">
-        <v>837.373293546117</v>
-      </c>
-      <c r="H19" s="16"/>
-      <c r="J19" s="28"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="51" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" s="37">
-        <v>89.8</v>
-      </c>
-      <c r="C20" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="D20" s="21">
-        <v>11900</v>
-      </c>
-      <c r="E20">
-        <v>7.63</v>
-      </c>
-      <c r="F20" s="54">
-        <v>740.03953883669703</v>
-      </c>
-      <c r="H20" s="16"/>
-      <c r="J20" s="16"/>
-    </row>
-    <row r="21" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="52" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="46">
-        <v>95</v>
-      </c>
-      <c r="C21" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="D21" s="22">
-        <v>12453</v>
-      </c>
-      <c r="E21" s="23">
-        <v>7.87</v>
-      </c>
-      <c r="F21" s="55">
-        <v>856.08018367798525</v>
-      </c>
-      <c r="H21" s="16"/>
-      <c r="J21" s="16"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Update demo input file
</commit_message>
<xml_diff>
--- a/data/GAMS_input_demo.xlsx
+++ b/data/GAMS_input_demo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chrishun\Box Sync\YSSP_temp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A488E5DA-74E0-43B0-A990-5BED5D190915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB260A6-0B3E-479B-9E49-ADBA58C13F15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3480" yWindow="-21720" windowWidth="38640" windowHeight="21390" tabRatio="705" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-2190" yWindow="-20430" windowWidth="28800" windowHeight="15555" tabRatio="705" firstSheet="13" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="1" r:id="rId1"/>
@@ -22,13 +22,13 @@
     <sheet name="virg_mat_supply" sheetId="8" r:id="rId7"/>
     <sheet name="mat_content" sheetId="9" r:id="rId8"/>
     <sheet name="mat_impact_int" sheetId="10" r:id="rId9"/>
-    <sheet name="batt_portfolio" sheetId="14" r:id="rId10"/>
+    <sheet name="component_portfolio" sheetId="14" r:id="rId10"/>
     <sheet name="newtec_int_shr" sheetId="2" r:id="rId11"/>
     <sheet name="eur_batt_share" sheetId="12" r:id="rId12"/>
     <sheet name="manuf_cnstrnt" sheetId="11" r:id="rId13"/>
     <sheet name="occupancy_rate" sheetId="3" r:id="rId14"/>
     <sheet name="tec_parameters_raw" sheetId="15" r:id="rId15"/>
-    <sheet name="enr_tec_correspondance" sheetId="16" r:id="rId16"/>
+    <sheet name="enr_tec_correspondence" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1323,8 +1323,8 @@
   </sheetPr>
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:R1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3321,8 +3321,8 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J47" sqref="J47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>